<commit_message>
Updated spreadsheet used for SmartSeq2 test.
</commit_message>
<xml_diff>
--- a/tests/fixtures/datasets/Smart-seq2/Q4DemoSS2Metadata_v5_plainHeaders_new.xlsx
+++ b/tests/fixtures/datasets/Smart-seq2/Q4DemoSS2Metadata_v5_plainHeaders_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrey/Development/hca/integration-tests/tests/fixtures/bundles/Smart-seq2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3FD41DFB-CD5C-8946-85C1-29D9E9E6CD63}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E69AE6F5-4335-7145-A388-459173D8B540}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32200" yWindow="-4920" windowWidth="41840" windowHeight="21560" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-10340" windowWidth="51200" windowHeight="28340" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="408">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -1249,6 +1249,9 @@
   </si>
   <si>
     <t>enrichment_protocol.enrichment_method.text</t>
+  </si>
+  <si>
+    <t>sequence_process_file_1</t>
   </si>
 </sst>
 </file>
@@ -2994,7 +2997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -3484,7 +3487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
@@ -3654,8 +3657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3821,6 +3824,9 @@
       <c r="J6" t="s">
         <v>385</v>
       </c>
+      <c r="L6" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
@@ -3843,6 +3849,9 @@
       </c>
       <c r="J7" t="s">
         <v>385</v>
+      </c>
+      <c r="L7" t="s">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>